<commit_message>
edits to p2 text doc and excel file
</commit_message>
<xml_diff>
--- a/Assignments/Assignment 3/Part 2 - User Evaluation/user data.xlsx
+++ b/Assignments/Assignment 3/Part 2 - User Evaluation/user data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18660" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>User</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Aurelié</t>
+  </si>
+  <si>
+    <t>T10</t>
   </si>
 </sst>
 </file>
@@ -218,9 +221,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -247,18 +250,21 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$J$3</c:f>
+              <c:f>Sheet1!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.0</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
@@ -279,10 +285,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -305,9 +314,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -334,16 +343,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$J$4</c:f>
+              <c:f>Sheet1!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -366,10 +378,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -392,9 +407,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -421,18 +436,21 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$J$5</c:f>
+              <c:f>Sheet1!$B$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
@@ -453,10 +471,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -479,9 +500,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -508,21 +529,24 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$J$6</c:f>
+              <c:f>Sheet1!$B$6:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
@@ -540,10 +564,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -566,9 +593,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -595,16 +622,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$J$7</c:f>
+              <c:f>Sheet1!$B$7:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -627,10 +657,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -647,11 +680,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2131483048"/>
-        <c:axId val="-2131486152"/>
+        <c:axId val="2066490936"/>
+        <c:axId val="2066493992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2131483048"/>
+        <c:axId val="2066490936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +693,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131486152"/>
+        <c:crossAx val="2066493992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,7 +701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131486152"/>
+        <c:axId val="2066493992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +731,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131483048"/>
+        <c:crossAx val="2066490936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -780,9 +813,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -809,27 +842,30 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$J$11</c:f>
+              <c:f>Sheet1!$B$11:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11.0</c:v>
@@ -838,13 +874,16 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -867,9 +906,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -896,16 +935,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$J$12</c:f>
+              <c:f>Sheet1!$B$12:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>21.0</c:v>
                 </c:pt>
@@ -913,7 +955,7 @@
                   <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.0</c:v>
@@ -931,6 +973,9 @@
                   <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -954,9 +999,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -983,30 +1028,33 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$J$13</c:f>
+              <c:f>Sheet1!$B$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.0</c:v>
@@ -1019,6 +1067,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1041,9 +1092,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -1070,24 +1121,27 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$J$14</c:f>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.0</c:v>
@@ -1099,13 +1153,16 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,9 +1185,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>T1</c:v>
                 </c:pt>
@@ -1157,21 +1214,24 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$J$15</c:f>
+              <c:f>Sheet1!$B$15:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.0</c:v>
@@ -1180,7 +1240,7 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.0</c:v>
@@ -1192,6 +1252,9 @@
                   <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1209,11 +1272,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113583576"/>
-        <c:axId val="-2113584728"/>
+        <c:axId val="2067271224"/>
+        <c:axId val="2067274280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113583576"/>
+        <c:axId val="2067271224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1222,7 +1285,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113584728"/>
+        <c:crossAx val="2067274280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1230,7 +1293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113584728"/>
+        <c:axId val="2067274280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1260,7 +1323,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113583576"/>
+        <c:crossAx val="2067271224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1669,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1680,12 +1743,12 @@
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1716,13 +1779,16 @@
       <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1743,13 +1809,16 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1775,18 +1844,21 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1807,13 +1879,16 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1821,7 +1896,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1839,13 +1914,16 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1871,18 +1949,21 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1913,8 +1994,11 @@
       <c r="J10" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K10" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1922,13 +2006,13 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <v>11</v>
@@ -1937,7 +2021,7 @@
         <v>5</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11">
         <v>14</v>
@@ -1945,8 +2029,11 @@
       <c r="J11">
         <v>8</v>
       </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1957,7 +2044,7 @@
         <v>6</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1977,8 +2064,11 @@
       <c r="J12">
         <v>6</v>
       </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1986,16 +2076,16 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -2009,8 +2099,11 @@
       <c r="J13">
         <v>3</v>
       </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -2018,10 +2111,10 @@
         <v>20</v>
       </c>
       <c r="C14">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -2033,7 +2126,7 @@
         <v>4</v>
       </c>
       <c r="H14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I14">
         <v>10</v>
@@ -2041,8 +2134,11 @@
       <c r="J14">
         <v>6</v>
       </c>
+      <c r="K14">
+        <v>8</v>
+      </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2050,7 +2146,7 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -2059,7 +2155,7 @@
         <v>3</v>
       </c>
       <c r="F15">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15">
         <v>4</v>
@@ -2073,8 +2169,11 @@
       <c r="J15">
         <v>4</v>
       </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2083,20 +2182,20 @@
         <v>18.399999999999999</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:J16" si="0">(SUM(C11:C15)/5)</f>
-        <v>8.8000000000000007</v>
+        <f t="shared" ref="C16:K16" si="0">(SUM(C11:C15)/5)</f>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>5.4</v>
+        <v>6.6</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8.6</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -2111,6 +2210,10 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="J16">
+        <f t="shared" si="0"/>
+        <v>5.4</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
@@ -2120,8 +2223,8 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <f>SUM(B16:J16)/9</f>
-        <v>7.3111111111111127</v>
+        <f>SUM(B16:K16)/10</f>
+        <v>7.080000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:10">

</xml_diff>